<commit_message>
added new category api path
</commit_message>
<xml_diff>
--- a/Info/Api Paths.xlsx
+++ b/Info/Api Paths.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="49">
   <si>
     <t>path</t>
   </si>
@@ -152,6 +152,27 @@
   </si>
   <si>
     <t>category list</t>
+  </si>
+  <si>
+    <t>/category/update/:id</t>
+  </si>
+  <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>change the services in category</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>/category/delete/:id</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>delete a category</t>
   </si>
 </sst>
 </file>
@@ -507,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,6 +744,43 @@
       </c>
       <c r="F11" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>